<commit_message>
Update of LD 10
Update of LD 10
</commit_message>
<xml_diff>
--- a/Civilworks cost/LD/Time Extention Data -  Kishoregonj WD.xlsx
+++ b/Civilworks cost/LD/Time Extention Data -  Kishoregonj WD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>Sl No.</t>
   </si>
@@ -382,15 +382,80 @@
     <t>Date of 
 Completion</t>
   </si>
+  <si>
+    <t>KISH/26</t>
+  </si>
+  <si>
+    <t>HOBI/01</t>
+  </si>
+  <si>
+    <t>HOBI/02</t>
+  </si>
+  <si>
+    <t>HOBI/03</t>
+  </si>
+  <si>
+    <t>HOBI/04</t>
+  </si>
+  <si>
+    <t>HOBI/05</t>
+  </si>
+  <si>
+    <t>HOBI/06</t>
+  </si>
+  <si>
+    <t>1st Revised</t>
+  </si>
+  <si>
+    <t>NETR/01</t>
+  </si>
+  <si>
+    <t>NETR/02</t>
+  </si>
+  <si>
+    <t>NETR/03</t>
+  </si>
+  <si>
+    <t>NETR/04</t>
+  </si>
+  <si>
+    <t>NETR/05</t>
+  </si>
+  <si>
+    <t>NETR/06</t>
+  </si>
+  <si>
+    <t>NETR/07</t>
+  </si>
+  <si>
+    <t>NETR/08</t>
+  </si>
+  <si>
+    <t>SUNM/01</t>
+  </si>
+  <si>
+    <t>SUNM/02</t>
+  </si>
+  <si>
+    <t>SUNM/03</t>
+  </si>
+  <si>
+    <t>SUNM/04</t>
+  </si>
+  <si>
+    <t>SUNM/05</t>
+  </si>
+  <si>
+    <t>SUNM/06</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -458,12 +523,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -550,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,43 +633,62 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -635,10 +725,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -947,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A34" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B51"/>
     </sheetView>
   </sheetViews>
@@ -965,18 +1052,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1009,890 +1096,890 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="30">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="30">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="38">
         <v>43071</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="27" t="s">
+      <c r="I5" s="30"/>
+      <c r="J5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="27"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="30">
         <v>3</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="27" t="s">
+      <c r="I7" s="30"/>
+      <c r="J7" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="27"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="30">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="30"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="27" t="s">
+      <c r="I11" s="30"/>
+      <c r="J11" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="27"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="30">
         <v>6</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="27" t="s">
+      <c r="I13" s="30"/>
+      <c r="J13" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="27"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="30">
         <v>7</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="38">
         <v>43224</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="27" t="s">
+      <c r="I15" s="30"/>
+      <c r="J15" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="27"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
+      <c r="A17" s="30">
         <v>8</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="38">
         <v>43314</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="29">
         <v>43497</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="27" t="s">
+      <c r="I17" s="30"/>
+      <c r="J17" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="27"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="27"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23">
+      <c r="A20" s="30">
         <v>9</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="38">
         <v>43374</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
+      <c r="G20" s="26"/>
+      <c r="H20" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24" t="s">
+      <c r="I20" s="30"/>
+      <c r="J20" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="25"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
+      <c r="A23" s="30">
         <v>10</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="38">
         <v>43374</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
+      <c r="G23" s="26"/>
+      <c r="H23" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="27" t="s">
+      <c r="I23" s="30"/>
+      <c r="J23" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="27"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="27"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="34"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
+      <c r="A26" s="30">
         <v>11</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
+      <c r="G26" s="26"/>
+      <c r="H26" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="27" t="s">
+      <c r="I26" s="30"/>
+      <c r="J26" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="27"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="27"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="34"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="23">
+      <c r="A29" s="30">
         <v>12</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19" t="s">
+      <c r="G29" s="26"/>
+      <c r="H29" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="27" t="s">
+      <c r="I29" s="30"/>
+      <c r="J29" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="27"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="34"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="27"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="34"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
+      <c r="A32" s="30">
         <v>13</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19" t="s">
+      <c r="G32" s="26"/>
+      <c r="H32" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="23">
+      <c r="A35" s="30">
         <v>14</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="31">
+      <c r="D35" s="38">
         <v>43070</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
+      <c r="G35" s="26"/>
+      <c r="H35" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="27" t="s">
+      <c r="I35" s="30"/>
+      <c r="J35" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="27"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="27"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23">
+      <c r="A38" s="30">
         <v>15</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="31">
+      <c r="D38" s="38">
         <v>42887</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19" t="s">
+      <c r="G38" s="26"/>
+      <c r="H38" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I38" s="23"/>
-      <c r="J38" s="27" t="s">
+      <c r="I38" s="30"/>
+      <c r="J38" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="27"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="27"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="34"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23">
+      <c r="A41" s="30">
         <v>16</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="31">
+      <c r="D41" s="38">
         <v>42887</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19" t="s">
+      <c r="G41" s="26"/>
+      <c r="H41" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I41" s="23"/>
-      <c r="J41" s="27" t="s">
+      <c r="I41" s="30"/>
+      <c r="J41" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="27"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="A43" s="30">
         <v>17</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19" t="s">
+      <c r="G43" s="26"/>
+      <c r="H43" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="I43" s="23"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="30"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="37"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="30"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="23">
+      <c r="A46" s="30">
         <v>18</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="29">
         <v>43591</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19" t="s">
+      <c r="G46" s="26"/>
+      <c r="H46" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="30"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="37"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="30"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="37"/>
     </row>
     <row r="49" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23">
+      <c r="A49" s="30">
         <v>19</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19" t="s">
+      <c r="G49" s="26"/>
+      <c r="H49" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I49" s="19" t="s">
+      <c r="I49" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="J49" s="23"/>
+      <c r="J49" s="30"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="23"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="30"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="23"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="30"/>
     </row>
     <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -2098,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,337 +2196,772 @@
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="E3" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="13">
         <v>42750</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="E4" s="13"/>
+      <c r="G4" s="5">
+        <f>MIN(E23:E45)</f>
+        <v>43910</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="13">
         <v>43071</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="13">
         <v>42870</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="13">
         <v>43097</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="13">
         <v>43600</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="13">
         <v>43151</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="13">
         <v>43636</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="13">
         <v>43093</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="13">
         <v>43616</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="13">
         <v>43093</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="13">
         <v>43616</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="13">
         <v>43224</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="13">
         <v>43615</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="13">
         <v>43314</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="13">
         <v>43497</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="13">
         <v>43374</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="13">
         <v>43604</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="13">
         <v>43374</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="13">
         <v>43600</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="13">
         <v>42750</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="13">
         <v>43151</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="13">
         <v>43636</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="13">
         <v>43143</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="13">
         <v>43636</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="13">
         <v>43070</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="13">
         <v>43248</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>15</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="13">
         <v>42887</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="13">
         <v>42887</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>17</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="13">
         <v>42717</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="E20" s="13"/>
+      <c r="F20" s="39">
+        <f>D20+777</f>
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="13">
         <v>43090</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="13">
         <v>43591</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
         <v>19</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="13">
         <v>42724</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="13">
         <v>43220</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="7"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="13">
+        <v>43151</v>
+      </c>
+      <c r="D23" s="12">
+        <v>43636</v>
+      </c>
+      <c r="E23" s="13">
+        <v>43972</v>
+      </c>
+      <c r="F23" s="21">
+        <f>E23-D23</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="13">
+        <v>43454</v>
+      </c>
+      <c r="D25" s="12">
+        <v>44012</v>
+      </c>
+      <c r="E25" s="12">
+        <v>44347</v>
+      </c>
+      <c r="F25" s="22">
+        <f>E25-D25</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="13">
+        <v>43446</v>
+      </c>
+      <c r="D26" s="12">
+        <v>44012</v>
+      </c>
+      <c r="E26" s="12">
+        <v>44347</v>
+      </c>
+      <c r="F26" s="22">
+        <f t="shared" ref="F26:F38" si="0">E26-D26</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="13">
+        <v>43114</v>
+      </c>
+      <c r="D27" s="12">
+        <v>43585</v>
+      </c>
+      <c r="E27" s="12">
+        <v>43951</v>
+      </c>
+      <c r="F27" s="21">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="13">
+        <v>43146</v>
+      </c>
+      <c r="D28" s="12">
+        <v>43585</v>
+      </c>
+      <c r="E28" s="12">
+        <v>43951</v>
+      </c>
+      <c r="F28" s="21">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="13">
+        <v>43115</v>
+      </c>
+      <c r="D29" s="12">
+        <v>43585</v>
+      </c>
+      <c r="E29" s="12">
+        <v>43951</v>
+      </c>
+      <c r="F29" s="21">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="13">
+        <v>43114</v>
+      </c>
+      <c r="D30" s="12">
+        <v>43585</v>
+      </c>
+      <c r="E30" s="12">
+        <v>43951</v>
+      </c>
+      <c r="F30" s="21">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="13">
+        <v>43130</v>
+      </c>
+      <c r="D32" s="12">
+        <v>43554</v>
+      </c>
+      <c r="E32" s="12">
+        <v>44012</v>
+      </c>
+      <c r="F32" s="21">
+        <f t="shared" si="0"/>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="13">
+        <v>43243</v>
+      </c>
+      <c r="D33" s="12">
+        <v>43615</v>
+      </c>
+      <c r="E33" s="12">
+        <v>44012</v>
+      </c>
+      <c r="F33" s="21">
+        <f t="shared" si="0"/>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="13">
+        <v>43243</v>
+      </c>
+      <c r="D34" s="12">
+        <v>43646</v>
+      </c>
+      <c r="E34" s="12">
+        <v>44012</v>
+      </c>
+      <c r="F34" s="21">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="13">
+        <v>43485</v>
+      </c>
+      <c r="D35" s="12">
+        <v>43920</v>
+      </c>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="13">
+        <v>43479</v>
+      </c>
+      <c r="D36" s="12">
+        <v>43920</v>
+      </c>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="13">
+        <v>43502</v>
+      </c>
+      <c r="D37" s="12">
+        <v>43920</v>
+      </c>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="13">
+        <v>43130</v>
+      </c>
+      <c r="D38" s="12">
+        <v>43570</v>
+      </c>
+      <c r="E38" s="12">
+        <v>43910</v>
+      </c>
+      <c r="F38" s="21">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="13">
+        <v>43857</v>
+      </c>
+      <c r="D39" s="12">
+        <v>44377</v>
+      </c>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="13">
+        <v>43457</v>
+      </c>
+      <c r="D40" s="12">
+        <v>43998</v>
+      </c>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="13">
+        <v>43457</v>
+      </c>
+      <c r="D41" s="12">
+        <v>43998</v>
+      </c>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="13">
+        <v>43462</v>
+      </c>
+      <c r="D42" s="12">
+        <v>44007</v>
+      </c>
+      <c r="E42" s="12">
+        <v>44377</v>
+      </c>
+      <c r="F42" s="21">
+        <f t="shared" ref="F42" si="1">E42-D42</f>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="13">
+        <v>43453</v>
+      </c>
+      <c r="D43" s="12">
+        <v>43997</v>
+      </c>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="13">
+        <v>43533</v>
+      </c>
+      <c r="D44" s="12">
+        <v>44007</v>
+      </c>
+      <c r="E44" s="12">
+        <v>44284</v>
+      </c>
+      <c r="F44" s="21">
+        <f t="shared" ref="F44:F45" si="2">E44-D44</f>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="13">
+        <v>43487</v>
+      </c>
+      <c r="D45" s="12">
+        <v>44007</v>
+      </c>
+      <c r="E45" s="12">
+        <v>44284</v>
+      </c>
+      <c r="F45" s="21">
+        <f t="shared" si="2"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated IPC Distribution 2018-19
Updated IPC Distribution 2018-19
</commit_message>
<xml_diff>
--- a/Civilworks cost/LD/Time Extention Data -  Kishoregonj WD.xlsx
+++ b/Civilworks cost/LD/Time Extention Data -  Kishoregonj WD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -644,54 +644,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -712,6 +664,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,38 +1019,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A38" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A44" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -1093,36 +1093,36 @@
       <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="19"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -1132,37 +1132,37 @@
       <c r="C5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="23">
         <v>43071</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21" t="s">
         <v>62</v>
       </c>
       <c r="I5" s="18"/>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>3</v>
       </c>
@@ -1175,34 +1175,34 @@
       <c r="D7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21" t="s">
         <v>63</v>
       </c>
       <c r="I7" s="18"/>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="18"/>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>4</v>
       </c>
@@ -1215,32 +1215,32 @@
       <c r="D9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="21" t="s">
         <v>64</v>
       </c>
       <c r="I9" s="18"/>
-      <c r="J9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="18"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>5</v>
       </c>
@@ -1253,34 +1253,34 @@
       <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="18"/>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="22"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>6</v>
       </c>
@@ -1293,34 +1293,34 @@
       <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21" t="s">
         <v>65</v>
       </c>
       <c r="I13" s="18"/>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="18"/>
-      <c r="J14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>7</v>
       </c>
@@ -1330,37 +1330,37 @@
       <c r="C15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="23">
         <v>43224</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="21" t="s">
         <v>66</v>
       </c>
       <c r="I15" s="18"/>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>8</v>
       </c>
@@ -1370,49 +1370,49 @@
       <c r="C17" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="23">
         <v>43314</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="19">
         <v>43497</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="21"/>
+      <c r="H17" s="21" t="s">
         <v>67</v>
       </c>
       <c r="I17" s="18"/>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="22"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="22"/>
-    </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>9</v>
       </c>
@@ -1422,49 +1422,49 @@
       <c r="C20" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="23">
         <v>43374</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="21"/>
+      <c r="H20" s="21" t="s">
         <v>68</v>
       </c>
       <c r="I20" s="18"/>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="18"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="18"/>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>10</v>
       </c>
@@ -1474,49 +1474,49 @@
       <c r="C23" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="23">
         <v>43374</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14" t="s">
+      <c r="G23" s="21"/>
+      <c r="H23" s="21" t="s">
         <v>68</v>
       </c>
       <c r="I23" s="18"/>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="18"/>
-      <c r="J24" s="22"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J24" s="20"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="18"/>
-      <c r="J25" s="22"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="20"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>11</v>
       </c>
@@ -1529,46 +1529,46 @@
       <c r="D26" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="21" t="s">
         <v>68</v>
       </c>
       <c r="I26" s="18"/>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J27" s="20"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="18"/>
-      <c r="J28" s="22"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>12</v>
       </c>
@@ -1581,46 +1581,46 @@
       <c r="D29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14" t="s">
+      <c r="G29" s="21"/>
+      <c r="H29" s="21" t="s">
         <v>68</v>
       </c>
       <c r="I29" s="18"/>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
       <c r="I30" s="18"/>
-      <c r="J30" s="22"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="18"/>
-      <c r="J31" s="22"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>13</v>
       </c>
@@ -1633,44 +1633,44 @@
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14" t="s">
+      <c r="G32" s="21"/>
+      <c r="H32" s="21" t="s">
         <v>69</v>
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>14</v>
       </c>
@@ -1680,141 +1680,141 @@
       <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="23">
         <v>43070</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14" t="s">
+      <c r="G35" s="21"/>
+      <c r="H35" s="21" t="s">
         <v>69</v>
       </c>
       <c r="I35" s="18"/>
-      <c r="J35" s="22" t="s">
+      <c r="J35" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="18"/>
-      <c r="J36" s="22"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="18"/>
-      <c r="J37" s="22"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>15</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="23">
         <v>42887</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14" t="s">
+      <c r="G38" s="21"/>
+      <c r="H38" s="21" t="s">
         <v>70</v>
       </c>
       <c r="I38" s="18"/>
-      <c r="J38" s="22" t="s">
+      <c r="J38" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
       <c r="I39" s="18"/>
-      <c r="J39" s="22"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="18"/>
-      <c r="J40" s="22"/>
-    </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>16</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="23">
         <v>42887</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14" t="s">
+      <c r="G41" s="21"/>
+      <c r="H41" s="21" t="s">
         <v>70</v>
       </c>
       <c r="I41" s="18"/>
-      <c r="J41" s="22" t="s">
+      <c r="J41" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="18"/>
-      <c r="J42" s="22"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>17</v>
       </c>
@@ -1827,44 +1827,44 @@
       <c r="D43" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14" t="s">
+      <c r="G43" s="21"/>
+      <c r="H43" s="21" t="s">
         <v>71</v>
       </c>
       <c r="I43" s="18"/>
-      <c r="J43" s="25"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
       <c r="I44" s="18"/>
-      <c r="J44" s="25"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="18"/>
-      <c r="J45" s="25"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J45" s="26"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>18</v>
       </c>
@@ -1877,236 +1877,131 @@
       <c r="D46" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="24">
         <v>43591</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14" t="s">
+      <c r="G46" s="21"/>
+      <c r="H46" s="21" t="s">
         <v>71</v>
       </c>
       <c r="I46" s="18"/>
-      <c r="J46" s="25"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
       <c r="I47" s="18"/>
-      <c r="J47" s="25"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J47" s="26"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
       <c r="I48" s="18"/>
-      <c r="J48" s="25"/>
-    </row>
-    <row r="49" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="26"/>
+    </row>
+    <row r="49" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>19</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="21" t="s">
         <v>74</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14" t="s">
+      <c r="G49" s="21"/>
+      <c r="H49" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="I49" s="21" t="s">
         <v>73</v>
       </c>
       <c r="J49" s="18"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="15"/>
+      <c r="C50" s="28"/>
       <c r="D50" s="18"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
-      <c r="C51" s="16"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="18"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
       <c r="J51" s="18"/>
     </row>
-    <row r="52" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="191">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="I32:I34"/>
-    <mergeCell ref="J32:J34"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="H46:H48"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="H49:H51"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="I43:I45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="D49:D51"/>
@@ -2131,37 +2026,142 @@
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="D43:D45"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="H46:H48"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="H49:H51"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="I43:I45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
@@ -2176,24 +2176,24 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="6" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
@@ -2217,509 +2217,509 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>17</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="13">
         <v>42717</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="14">
         <v>43220</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="14">
         <v>43997</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="15">
         <f t="shared" ref="G4:G22" si="0">F4-E4</f>
         <v>777</v>
       </c>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>11</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="13">
         <v>42750</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="14">
         <v>43220</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="14">
         <v>43982</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="15">
         <f t="shared" si="0"/>
         <v>762</v>
       </c>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>15</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="13">
         <v>42887</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="14">
         <v>43220</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="14">
         <v>43921</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="15">
         <f t="shared" si="0"/>
         <v>701</v>
       </c>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="13">
         <v>42750</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="14">
         <v>43220</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="14">
         <v>43905</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="15">
         <f t="shared" si="0"/>
         <v>685</v>
       </c>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>19</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="13">
         <v>42724</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="14">
         <v>43220</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="14">
         <v>43610</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="15">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="13">
         <v>43071</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="14">
         <v>42870</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="14">
         <v>43982</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="15">
         <f t="shared" si="0"/>
         <v>1112</v>
       </c>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="13">
         <v>43374</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="14">
         <v>43604</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="14">
         <v>43951</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="15">
         <f t="shared" si="0"/>
         <v>347</v>
       </c>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>5</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="13">
         <v>43093</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="14">
         <v>43616</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="14">
         <v>43972</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="15">
         <f t="shared" si="0"/>
         <v>356</v>
       </c>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>6</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="13">
         <v>43093</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="14">
         <v>43616</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="14">
         <v>43972</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="15">
         <f t="shared" si="0"/>
         <v>356</v>
       </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>13</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="13">
         <v>43143</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="14">
         <v>43636</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="14">
         <v>44042</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="15">
         <f t="shared" si="0"/>
         <v>406</v>
       </c>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>16</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="13">
         <v>42887</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="14">
         <v>43220</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="14">
         <v>43982</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="15">
         <f t="shared" si="0"/>
         <v>762</v>
       </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="27">
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="13">
         <v>43070</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="14">
         <v>43248</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="14">
         <v>43976</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="15">
         <f t="shared" si="0"/>
         <v>728</v>
       </c>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>10</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="13">
         <v>43374</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="14">
         <v>43600</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="14">
         <v>43982</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="15">
         <f t="shared" si="0"/>
         <v>382</v>
       </c>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="27">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>3</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="13">
         <v>43097</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="14">
         <v>43600</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="14">
         <v>43982</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="15">
         <f t="shared" si="0"/>
         <v>382</v>
       </c>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>8</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="13">
         <v>43314</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="14">
         <v>43497</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="14">
         <v>43921</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="15">
         <f t="shared" si="0"/>
         <v>424</v>
       </c>
-      <c r="H18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="27">
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
         <v>4</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="13">
         <v>43151</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="14">
         <v>43636</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="14">
         <v>44027</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="15">
         <f t="shared" si="0"/>
         <v>391</v>
       </c>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="27">
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>7</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="13">
         <v>43224</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="14">
         <v>43615</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="14">
         <v>43982</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="15">
         <f t="shared" si="0"/>
         <v>367</v>
       </c>
-      <c r="H20" s="30"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="27">
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
         <v>18</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="13">
         <v>43090</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="14">
         <v>43591</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="14">
         <v>43997</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="15">
         <f t="shared" si="0"/>
         <v>406</v>
       </c>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="32">
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>12</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="13">
         <v>43151</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="14">
         <v>43636</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="14">
         <v>43972</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="15">
         <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D32" s="5"/>
     </row>
   </sheetData>

</xml_diff>